<commit_message>
Did truth and equality exercises
</commit_message>
<xml_diff>
--- a/Learning-Overview.xlsx
+++ b/Learning-Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ademir Alijagic\Documents\GitHub\AW-program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A0EAEC-E470-4803-87D1-09620E6CC861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74647E26-5EA4-4C44-9E17-5EF511C270C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4910" yWindow="-70" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Module-1-JS-Programming-Fundamentals-and-Problem-Solving-Using-Code</t>
   </si>
@@ -183,6 +183,39 @@
   </si>
   <si>
     <t>Palindrome</t>
+  </si>
+  <si>
+    <t>3-1-1-Basic Syntax</t>
+  </si>
+  <si>
+    <t>3-1-2-Types and Literals</t>
+  </si>
+  <si>
+    <t>3-1-3-Truth and Equality</t>
+  </si>
+  <si>
+    <t>3-2-1-Objects</t>
+  </si>
+  <si>
+    <t>3-2-2-Classes</t>
+  </si>
+  <si>
+    <t>3-2-3-Functions</t>
+  </si>
+  <si>
+    <t>3-3-1-Closures</t>
+  </si>
+  <si>
+    <t>3-3-2-Composition</t>
+  </si>
+  <si>
+    <t>3-3-3-Array Methods</t>
+  </si>
+  <si>
+    <t>3-4-1-Array Reducing</t>
+  </si>
+  <si>
+    <t>3-4-2-This</t>
   </si>
 </sst>
 </file>
@@ -388,7 +421,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -412,7 +445,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -692,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1059,18 +1092,18 @@
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -1084,18 +1117,18 @@
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
@@ -1109,18 +1142,18 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -1134,18 +1167,18 @@
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -1159,18 +1192,18 @@
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -1184,18 +1217,18 @@
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -1209,18 +1242,18 @@
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1255,20 +1288,295 @@
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
     </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:U5 B7:U91 B6:C6 G6:I6 K6:U6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Confident"</formula>
+  <conditionalFormatting sqref="B4:U5 B6:C6 G6:I6 K6:U6 B7:U90">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Not Started"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Learning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Started"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Confident"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>